<commit_message>
[general] - set limit on Excel cell width expansion. MS Excel only support 255 as maximum for cell width.
[base]
- reduce some of more "cryptic" console output passed down from Selenium 2 implementation.

[json]
- [`assertValues(json,jsonpath,array,exactOrder)`](../commands/json/assertValues(json,jsonpath,array,exactOrder)):
  enhanced to support better comparison-equivalent logic (like that of
  [`assertEqual(expected,actual)`](../commands/json/assertEqual(expected,actual))).

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_json.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_json.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11014"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F8A7AA-C4F2-9D43-BFC8-253D3E70EDCF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C209AD8-172E-4946-93D9-48E8EDFA4884}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="10960" windowWidth="41920" windowHeight="21040" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
     <definedName name="ws.async">'#system'!$Y$2:$Y$8</definedName>
     <definedName name="xml">'#system'!$Z$2:$Z$11</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="592">
   <si>
     <t>description</t>
   </si>
@@ -1842,6 +1842,40 @@
   </si>
   <si>
     <t>[]</t>
+  </si>
+  <si>
+    <t>Asset Object Array</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/unitTest_json_doc3.json</t>
+  </si>
+  <si>
+    <t>jobParameters</t>
+  </si>
+  <si>
+    <t>response.jobParameters</t>
+  </si>
+  <si>
+    <t>val1</t>
+  </si>
+  <si>
+    <t>${val1}</t>
+  </si>
+  <si>
+    <t>${jobParameters}</t>
+  </si>
+  <si>
+    <t>[JSON(${jobParameters}) =&gt; pack text]</t>
+  </si>
+  <si>
+    <t>[JSON(${val1}) =&gt; pack text]</t>
+  </si>
+  <si>
+    <t>[{
+      "parameterName": "summaryId",
+      "parameterValue": "123456",
+      "parameterType": "QUERY"
+    }]</t>
   </si>
 </sst>
 </file>
@@ -4208,10 +4242,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O1000"/>
+  <dimension ref="A1:O998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5039,12 +5073,22 @@
       <c r="O30" s="3"/>
     </row>
     <row r="31" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="27"/>
+      <c r="A31" s="27" t="s">
+        <v>582</v>
+      </c>
       <c r="B31" s="5"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="C31" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>583</v>
+      </c>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
@@ -5055,13 +5099,21 @@
       <c r="N31" s="15"/>
       <c r="O31" s="3"/>
     </row>
-    <row r="32" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="80" x14ac:dyDescent="0.2">
       <c r="A32" s="27"/>
       <c r="B32" s="5"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="C32" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>584</v>
+      </c>
+      <c r="F32" s="22" t="s">
+        <v>591</v>
+      </c>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
@@ -5075,11 +5127,21 @@
     <row r="33" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="27"/>
       <c r="B33" s="5"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
+      <c r="C33" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>585</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>586</v>
+      </c>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
       <c r="J33" s="22"/>
@@ -5092,10 +5154,18 @@
     <row r="34" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="27"/>
       <c r="B34" s="5"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
+      <c r="C34" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>589</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>590</v>
+      </c>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
@@ -5109,10 +5179,18 @@
     <row r="35" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="27"/>
       <c r="B35" s="5"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
+      <c r="C35" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>588</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>587</v>
+      </c>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
@@ -5126,12 +5204,24 @@
     <row r="36" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="27"/>
       <c r="B36" s="5"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
+      <c r="C36" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>585</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>588</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>384</v>
+      </c>
       <c r="I36" s="7"/>
       <c r="J36" s="22"/>
       <c r="K36" s="3"/>
@@ -5514,7 +5604,7 @@
       <c r="N58" s="15"/>
       <c r="O58" s="3"/>
     </row>
-    <row r="59" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="27"/>
       <c r="B59" s="5"/>
       <c r="C59" s="13"/>
@@ -5531,7 +5621,7 @@
       <c r="N59" s="15"/>
       <c r="O59" s="3"/>
     </row>
-    <row r="60" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="27"/>
       <c r="B60" s="5"/>
       <c r="C60" s="13"/>
@@ -15510,40 +15600,8 @@
       <c r="N646" s="15"/>
       <c r="O646" s="3"/>
     </row>
-    <row r="647" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A647" s="27"/>
-      <c r="B647" s="5"/>
-      <c r="C647" s="13"/>
-      <c r="D647" s="7"/>
-      <c r="E647" s="7"/>
-      <c r="F647" s="7"/>
-      <c r="G647" s="7"/>
-      <c r="H647" s="7"/>
-      <c r="I647" s="7"/>
-      <c r="J647" s="22"/>
-      <c r="K647" s="3"/>
-      <c r="L647" s="15"/>
-      <c r="M647" s="12"/>
-      <c r="N647" s="15"/>
-      <c r="O647" s="3"/>
-    </row>
-    <row r="648" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A648" s="27"/>
-      <c r="B648" s="5"/>
-      <c r="C648" s="13"/>
-      <c r="D648" s="7"/>
-      <c r="E648" s="7"/>
-      <c r="F648" s="7"/>
-      <c r="G648" s="7"/>
-      <c r="H648" s="7"/>
-      <c r="I648" s="7"/>
-      <c r="J648" s="22"/>
-      <c r="K648" s="3"/>
-      <c r="L648" s="15"/>
-      <c r="M648" s="12"/>
-      <c r="N648" s="15"/>
-      <c r="O648" s="3"/>
-    </row>
+    <row r="647" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="648" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="649" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="650" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="651" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -15894,8 +15952,6 @@
     <row r="996" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="997" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection insertRows="0" insertHyperlinks="0" deleteRows="0"/>
   <mergeCells count="4">
@@ -15916,10 +15972,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D698" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D696" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C700" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C698" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>target</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[json commands] - [`assertEquals(expected,actual)`]: fixed inefficient and confusing comparison logic when `expected` and `actual` do not have the same nodes or node names. - [`assertEquals(expected,actual)`]: add new System variable to support CSV and HTML report format:   - [`nexial.json.compareResultsAsJSON`]: `true` (default) to generate comparison result as JSON.   - [`nexial.json.compareResultsAsCSV`]: `true` (default is `false`) to generate comparison result as CSV.   - [`nexial.json.compareResultsAsHTML`]: `true` (default is `false`) to generate comparison result as HTML.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_json.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_json.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD9EA73-51DC-3040-BEA8-EB3A818CA98E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E512B477-7F68-BA40-898D-616A5C0A814A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="57600" windowHeight="17760" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="704">
   <si>
     <t>description</t>
   </si>
@@ -2215,9 +2215,6 @@
   </si>
   <si>
     <t>false</t>
-  </si>
-  <si>
-    <t>open ${nexial.lastOutputLink}</t>
   </si>
   <si>
     <t>css file</t>
@@ -2526,6 +2523,14 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -2553,14 +2558,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4986,12 +4983,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="24" t="s">
         <v>11</v>
       </c>
@@ -5009,20 +5006,20 @@
       </c>
       <c r="J1" s="19"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="39"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="41"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
       <c r="E2" s="25"/>
       <c r="F2" s="26"/>
       <c r="G2" s="25"/>
@@ -5032,10 +5029,10 @@
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
@@ -16729,12 +16726,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="29" t="s">
         <v>11</v>
       </c>
@@ -16752,20 +16749,20 @@
       </c>
       <c r="J1" s="19"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="39"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="41"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
       <c r="E2" s="25"/>
       <c r="F2" s="26"/>
       <c r="G2" s="25"/>
@@ -16775,10 +16772,10 @@
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
@@ -28364,7 +28361,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -28387,12 +28384,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="30" t="s">
         <v>11</v>
       </c>
@@ -28410,20 +28407,20 @@
       </c>
       <c r="J1" s="19"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="39"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="41"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
       <c r="E2" s="25"/>
       <c r="F2" s="26"/>
       <c r="G2" s="25"/>
@@ -28433,10 +28430,10 @@
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
@@ -29062,10 +29059,10 @@
       <c r="D26" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E26" s="42" t="s">
+      <c r="E26" s="34" t="s">
         <v>693</v>
       </c>
-      <c r="F26" s="42" t="s">
+      <c r="F26" s="34" t="s">
         <v>380</v>
       </c>
       <c r="G26" s="7"/>
@@ -29087,10 +29084,10 @@
       <c r="D27" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E27" s="42" t="s">
+      <c r="E27" s="34" t="s">
         <v>694</v>
       </c>
-      <c r="F27" s="42" t="s">
+      <c r="F27" s="34" t="s">
         <v>380</v>
       </c>
       <c r="G27" s="7"/>
@@ -29163,10 +29160,10 @@
         <v>81</v>
       </c>
       <c r="E30" s="10" t="s">
+        <v>701</v>
+      </c>
+      <c r="F30" s="7" t="s">
         <v>702</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>703</v>
       </c>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
@@ -29190,8 +29187,8 @@
       <c r="E31" s="7" t="s">
         <v>695</v>
       </c>
-      <c r="F31" s="43" t="s">
-        <v>704</v>
+      <c r="F31" s="35" t="s">
+        <v>703</v>
       </c>
       <c r="G31" s="7" t="s">
         <v>700</v>
@@ -29208,15 +29205,9 @@
     <row r="32" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="27"/>
       <c r="B32" s="5"/>
-      <c r="C32" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>620</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>701</v>
-      </c>
+      <c r="C32" s="13"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
@@ -40129,12 +40120,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="31" t="s">
         <v>11</v>
       </c>
@@ -40152,20 +40143,20 @@
       </c>
       <c r="J1" s="19"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="39"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="41"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="38" t="s">
         <v>564</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
       <c r="E2" s="25"/>
       <c r="F2" s="26"/>
       <c r="G2" s="25"/>
@@ -40175,10 +40166,10 @@
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
@@ -51643,12 +51634,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="33" t="s">
         <v>11</v>
       </c>
@@ -51666,20 +51657,20 @@
       </c>
       <c r="J1" s="19"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="39"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="41"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="38" t="s">
         <v>564</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
       <c r="E2" s="25"/>
       <c r="F2" s="26"/>
       <c r="G2" s="25"/>
@@ -51689,10 +51680,10 @@
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>

</xml_diff>